<commit_message>
Atualização da Lista de Riscos
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Magnitude</t>
   </si>
@@ -164,6 +164,27 @@
   </si>
   <si>
     <t>Documentar todos os requisitos recebidos dos Stakeholder´s e os manter sempre informados sobre os impactos sofridos no desenvolvimento de acordo com a sua nova expectativa.</t>
+  </si>
+  <si>
+    <t>É possível que ocorram problemas diversos com o fornecimento de energia elétrica. Este problema pode afetar não apenas o desenvolvimento, como também a queima de equipamentos diversos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fornecimento de energia elétrica ininterrupta para todos os equipamentos que serão utilizados pela a equipe de desenvolvimento de software. </t>
+  </si>
+  <si>
+    <t>Gerente de Configuração e Mudança.</t>
+  </si>
+  <si>
+    <t>Contratar empresa de locação de Gerador Elétrico e que será responsável também pela prestação de serviço de instalação e manutenção do mesmo.</t>
+  </si>
+  <si>
+    <t>Queima de equipamentos diversos que serão utilizados pela a equipe de desenvolvimento de software</t>
+  </si>
+  <si>
+    <t>Pode ser necessário realizarmos o conserto ou substituição de equipamentos que vierem a apresentar defeitos.</t>
+  </si>
+  <si>
+    <t>Contratar empresa de manutenção para os equipamentos elétrico/eletrônicos que serão utilizados por toda a equipe de desenvolvimento de software.</t>
   </si>
 </sst>
 </file>
@@ -644,7 +665,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -686,7 +707,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -712,7 +733,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -725,7 +746,7 @@
     <col min="6" max="6" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="36.140625" style="2" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -772,7 +793,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>41934</v>
+        <v>41842</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
@@ -805,7 +826,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>41900</v>
+        <v>41869</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>16</v>
@@ -838,7 +859,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>41902</v>
+        <v>41871</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>19</v>
@@ -871,7 +892,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>41824</v>
+        <v>41886</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>26</v>
@@ -899,39 +920,71 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1">
+    <row r="7" spans="1:10" s="9" customFormat="1" ht="75.75" customHeight="1">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="7"/>
+      <c r="B7" s="6">
+        <v>41888</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.2</v>
+      </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" s="9" customFormat="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="9" customFormat="1" ht="63.75">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="7"/>
+      <c r="B8" s="6">
+        <v>41894</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.05</v>
+      </c>
       <c r="H8" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:10" s="9" customFormat="1">
       <c r="A9" s="3">

</xml_diff>

<commit_message>
Atualizações diversas (Feedback Professor Jarley)
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -665,7 +665,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -707,7 +707,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -733,7 +733,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Atualização de documentos Visão, Risco, Iteração
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -246,7 +246,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -269,25 +269,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -324,24 +311,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
@@ -665,7 +634,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -707,7 +676,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -730,10 +699,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -757,7 +726,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="82.5" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -769,19 +738,19 @@
       <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="12" t="s">
@@ -844,7 +813,7 @@
         <v>0.5</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" ref="H4:H20" si="0">+F4*G4</f>
+        <f t="shared" ref="H4:H12" si="0">+F4*G4</f>
         <v>2.5</v>
       </c>
       <c r="I4" s="8" t="s">
@@ -1053,142 +1022,6 @@
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" s="9" customFormat="1">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" spans="1:10" s="9" customFormat="1">
-      <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" s="9" customFormat="1">
-      <c r="A15" s="3">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" s="9" customFormat="1">
-      <c r="A16" s="3">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" s="9" customFormat="1">
-      <c r="A17" s="3">
-        <v>15</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" s="9" customFormat="1">
-      <c r="A18" s="3">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" s="9" customFormat="1">
-      <c r="A19" s="3">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" s="9" customFormat="1">
-      <c r="A20" s="3">
-        <v>18</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Correção documentos diversos (Feedback do Professor)
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -194,11 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -270,54 +266,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -634,7 +619,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -676,7 +661,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -699,10 +684,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -721,47 +706,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="82.5" customHeight="1">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="82.5" customHeight="1">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="9" customFormat="1" ht="38.25">
+    <row r="3" spans="1:10" s="8" customFormat="1" ht="38.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>41842</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -776,25 +761,25 @@
       <c r="F3" s="3">
         <v>5</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>0.1</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <f>+F3*G3</f>
         <v>0.5</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="9" customFormat="1" ht="54" customHeight="1">
+    <row r="4" spans="1:10" s="8" customFormat="1" ht="54" customHeight="1">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>41869</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -809,25 +794,25 @@
       <c r="F4" s="3">
         <v>5</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>0.5</v>
       </c>
-      <c r="H4" s="8">
-        <f t="shared" ref="H4:H12" si="0">+F4*G4</f>
+      <c r="H4" s="7">
+        <f t="shared" ref="H4:H8" si="0">+F4*G4</f>
         <v>2.5</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="9" customFormat="1" ht="68.25" customHeight="1">
+    <row r="5" spans="1:10" s="8" customFormat="1" ht="68.25" customHeight="1">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>41871</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -842,25 +827,25 @@
       <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>0.05</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="9" customFormat="1" ht="86.25" customHeight="1">
+    <row r="6" spans="1:10" s="8" customFormat="1" ht="86.25" customHeight="1">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>41886</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -875,25 +860,25 @@
       <c r="F6" s="3">
         <v>3</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>0.7</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" ht="75.75" customHeight="1">
+    <row r="7" spans="1:10" s="8" customFormat="1" ht="75.75" customHeight="1">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>41888</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -908,25 +893,25 @@
       <c r="F7" s="3">
         <v>5</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>0.2</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="9" customFormat="1" ht="63.75">
+    <row r="8" spans="1:10" s="8" customFormat="1" ht="63.75">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>41894</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -941,87 +926,19 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>0.05</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="9" customFormat="1">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" s="9" customFormat="1">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" s="9" customFormat="1">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" s="9" customFormat="1">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
1º Commit de correções conf. feedback Professor
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -115,9 +115,6 @@
     <t>Lista de Riscos: Projeto Sistema de Rastreamento</t>
   </si>
   <si>
-    <t>Problema na contratação do Data Center</t>
-  </si>
-  <si>
     <t>O contrato pode não ser concretizado</t>
   </si>
   <si>
@@ -130,18 +127,12 @@
     <t>Realizar 03 cotações diferentes e definir o primeiro e segundo colocado.</t>
   </si>
   <si>
-    <t>Programador com domínio pleno nas duas linguagens principais PHP e Java utilizadas no sistema</t>
-  </si>
-  <si>
     <t>O programador pode ter dificuldades na solução de um deter,minado pacote de trabalho em uma linguagem específica</t>
   </si>
   <si>
     <t>Contratar no formato Free Lance um especialista para cada linguagem específica deixando-o de sobre aviso.</t>
   </si>
   <si>
-    <t>Realizar correções na aplicação principal não previstas e muito frequentes</t>
-  </si>
-  <si>
     <t>Fatores externos podem vir a prejudicar o desenvolvimento da aplicação, ocasionando um número inesperado de correções.</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
     <t>Analista de Desenvolvimento</t>
   </si>
   <si>
-    <t>Mudança na expectativa dos Stakeholder´s quanto às funcionalidades do Sistema de Rastreamento</t>
-  </si>
-  <si>
     <t>Documentar todos os requisitos recebidos dos Stakeholder´s e os manter sempre informados sobre os impactos sofridos no desenvolvimento de acordo com a sua nova expectativa.</t>
   </si>
   <si>
@@ -178,13 +166,25 @@
     <t>Contratar empresa de locação de Gerador Elétrico e que será responsável também pela prestação de serviço de instalação e manutenção do mesmo.</t>
   </si>
   <si>
-    <t>Queima de equipamentos diversos que serão utilizados pela a equipe de desenvolvimento de software</t>
-  </si>
-  <si>
     <t>Pode ser necessário realizarmos o conserto ou substituição de equipamentos que vierem a apresentar defeitos.</t>
   </si>
   <si>
     <t>Contratar empresa de manutenção para os equipamentos elétrico/eletrônicos que serão utilizados por toda a equipe de desenvolvimento de software.</t>
+  </si>
+  <si>
+    <t>Problema na contratação do Data Center.</t>
+  </si>
+  <si>
+    <t>Programador com domínio pleno nas duas linguagens principais PHP e Java utilizadas no sistema.</t>
+  </si>
+  <si>
+    <t>Mudança na expectativa dos Stakeholder´s quanto às funcionalidades do Sistema de Rastreamento.</t>
+  </si>
+  <si>
+    <t>Realizar correções na aplicação principal não previstas e muito frequentes.</t>
+  </si>
+  <si>
+    <t>Queima de equipamentos diversos que serão utilizados pela a equipe de desenvolvimento de software.</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -661,7 +661,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -686,8 +686,8 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -750,13 +750,13 @@
         <v>41842</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="F3" s="3">
         <v>5</v>
@@ -769,10 +769,10 @@
         <v>0.5</v>
       </c>
       <c r="I3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="8" customFormat="1" ht="54" customHeight="1">
@@ -783,13 +783,13 @@
         <v>41869</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3">
         <v>5</v>
@@ -802,10 +802,10 @@
         <v>2.5</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="8" customFormat="1" ht="68.25" customHeight="1">
@@ -816,13 +816,13 @@
         <v>41871</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -835,10 +835,10 @@
         <v>0.1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="86.25" customHeight="1">
@@ -849,13 +849,13 @@
         <v>41886</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3">
         <v>3</v>
@@ -868,10 +868,10 @@
         <v>2.0999999999999996</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" ht="75.75" customHeight="1">
@@ -882,13 +882,13 @@
         <v>41888</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="3">
         <v>5</v>
@@ -901,10 +901,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" ht="63.75">
@@ -915,13 +915,13 @@
         <v>41894</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -934,10 +934,10 @@
         <v>0.05</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de documentos diversos
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -619,7 +619,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -661,7 +661,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>

</xml_diff>

<commit_message>
Correção Risk List e Work Items List
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -133,27 +133,15 @@
     <t>Contratar no formato Free Lance um especialista para cada linguagem específica deixando-o de sobre aviso.</t>
   </si>
   <si>
-    <t>Fatores externos podem vir a prejudicar o desenvolvimento da aplicação, ocasionando um número inesperado de correções.</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
     <t>Analista de testes</t>
   </si>
   <si>
-    <t>Contratar um especialista da área de desenvolvimento de software que ficará alocado apenas para prospectar as inovações e/ou necessidades do mercado.</t>
-  </si>
-  <si>
-    <t>Necessidades diferentes das que foram identificadas no início do projeto podem vir a ocorrer</t>
-  </si>
-  <si>
     <t>Analista de Desenvolvimento</t>
   </si>
   <si>
-    <t>Documentar todos os requisitos recebidos dos Stakeholder´s e os manter sempre informados sobre os impactos sofridos no desenvolvimento de acordo com a sua nova expectativa.</t>
-  </si>
-  <si>
     <t>É possível que ocorram problemas diversos com o fornecimento de energia elétrica. Este problema pode afetar não apenas o desenvolvimento, como também a queima de equipamentos diversos.</t>
   </si>
   <si>
@@ -178,13 +166,25 @@
     <t>Programador com domínio pleno nas duas linguagens principais PHP e Java utilizadas no sistema.</t>
   </si>
   <si>
-    <t>Mudança na expectativa dos Stakeholder´s quanto às funcionalidades do Sistema de Rastreamento.</t>
-  </si>
-  <si>
-    <t>Realizar correções na aplicação principal não previstas e muito frequentes.</t>
-  </si>
-  <si>
     <t>Queima de equipamentos diversos que serão utilizados pela a equipe de desenvolvimento de software.</t>
+  </si>
+  <si>
+    <t>Problemas de infraestrutura/rede na instalação de aplicativos, configuração e/ou manutenção no Datacenter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificamos a necessidade de um profissional para solução de possíveis problemas de infraestrutura/redes no Datacenter. </t>
+  </si>
+  <si>
+    <t>Contratar profissional de infraestrutura/redes em regime CLT.</t>
+  </si>
+  <si>
+    <t>Contratar um especialista da área de desenvolvimento de software que ficará alocado apenas para prospectar as inovações e/ou mudanças no mercado.</t>
+  </si>
+  <si>
+    <t>Realizar correções/atualizações na aplicação principal não previstas devido a possíveis mudanças de mercado.</t>
+  </si>
+  <si>
+    <t>Fatores externos podem vir a prejudicar o desenvolvimento da aplicação, ocasionando correções inesperadas no projeto e que podem comprometer a qualidade final.</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -661,7 +661,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -686,8 +686,8 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -750,7 +750,7 @@
         <v>41842</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -783,7 +783,7 @@
         <v>41869</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>15</v>
@@ -819,10 +819,10 @@
         <v>33</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -835,10 +835,10 @@
         <v>0.1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="86.25" customHeight="1">
@@ -849,29 +849,29 @@
         <v>41886</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G6" s="6">
         <v>0.7</v>
       </c>
       <c r="H6" s="7">
         <f t="shared" si="0"/>
-        <v>2.0999999999999996</v>
+        <v>3.5</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" ht="75.75" customHeight="1">
@@ -882,10 +882,10 @@
         <v>41888</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>12</v>
@@ -901,10 +901,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" ht="63.75">
@@ -915,13 +915,13 @@
         <v>41894</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -934,10 +934,10 @@
         <v>0.05</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diagrama de Classes, Sequência e Projeto Arquitetural
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -619,7 +619,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -661,7 +661,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -686,8 +686,8 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -762,11 +762,11 @@
         <v>5</v>
       </c>
       <c r="G3" s="6">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="H3" s="7">
         <f>+F3*G3</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>13</v>
@@ -795,11 +795,11 @@
         <v>5</v>
       </c>
       <c r="G4" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" ref="H4:H8" si="0">+F4*G4</f>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>13</v>
@@ -861,11 +861,11 @@
         <v>5</v>
       </c>
       <c r="G6" s="6">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="H6" s="7">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>19</v>
@@ -894,11 +894,11 @@
         <v>5</v>
       </c>
       <c r="G7" s="6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Disponibilização de modelos para Edson
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Magnitude</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Fatores externos podem vir a prejudicar o desenvolvimento da aplicação, ocasionando correções inesperadas no projeto e que podem comprometer a qualidade final.</t>
+  </si>
+  <si>
+    <t>Risco novo de integração/novo componente na equipe</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -299,6 +302,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,7 +625,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -661,7 +667,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -684,10 +690,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -940,6 +946,11 @@
         <v>25</v>
       </c>
     </row>
+    <row r="10" spans="1:10" ht="25.5">
+      <c r="C10" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Remoção Templates e Inserção novos documentos
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Magnitude</t>
   </si>
@@ -187,7 +187,13 @@
     <t>Fatores externos podem vir a prejudicar o desenvolvimento da aplicação, ocasionando correções inesperadas no projeto e que podem comprometer a qualidade final.</t>
   </si>
   <si>
-    <t>Risco novo de integração/novo componente na equipe</t>
+    <t>Risco de integração de um novo componente na equipe</t>
+  </si>
+  <si>
+    <t>Será necessário realizarmos um treinamento para o novo integrante da equipe</t>
+  </si>
+  <si>
+    <t>Realizar treinamentos com carga horária de 4 horas diárias, de forma individual, realizada por cada integrante da equipe de desenvolvimento.</t>
   </si>
 </sst>
 </file>
@@ -245,7 +251,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -268,11 +274,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -304,6 +321,19 @@
       <alignment textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -625,7 +655,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -667,7 +697,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -690,10 +720,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -704,7 +734,7 @@
     <col min="4" max="4" width="35.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="3.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="12.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="36.140625" style="2" customWidth="1"/>
@@ -804,7 +834,7 @@
         <v>0.05</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="H4:H8" si="0">+F4*G4</f>
+        <f t="shared" ref="H4:H9" si="0">+F4*G4</f>
         <v>0.25</v>
       </c>
       <c r="I4" s="7" t="s">
@@ -946,9 +976,37 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25.5">
-      <c r="C10" s="12" t="s">
+    <row r="9" spans="1:10" ht="63.75">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="14">
+        <v>41716</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>35</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="13">
+        <v>3</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="H9" s="16">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizar Lista de ìtens de trabalho e risco
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Magnitude</t>
   </si>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>Realizar cópia mais atual do banco de dados e disponibilizar para testes.</t>
+  </si>
+  <si>
+    <t>Risco da falta de domínio nos padrões de UML pode gerar problemas na equipe no desenvolvimento da aplicação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar treinamento sobre o padrão UMLcom todos os integrantes da equipe de desenvolvimento </t>
+  </si>
+  <si>
+    <t>Organizar os treinamentos aos Sábados para não gerar aumento de custo significativo ao projeto</t>
   </si>
 </sst>
 </file>
@@ -667,7 +676,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -709,7 +718,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -732,10 +741,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -846,7 +855,7 @@
         <v>0.05</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="H4:H10" si="0">+F4*G4</f>
+        <f t="shared" ref="H4:H11" si="0">+F4*G4</f>
         <v>0.25</v>
       </c>
       <c r="I4" s="7" t="s">
@@ -1052,6 +1061,36 @@
       </c>
       <c r="J10" s="17" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="38.25">
+      <c r="B11" s="14">
+        <v>41739</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="13">
+        <v>3</v>
+      </c>
+      <c r="G11" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="H11" s="16">
+        <f t="shared" si="0"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização de lista de riscos.
como está se aproximando a entrega final, froam descobertos novos
riscos.
</commit_message>
<xml_diff>
--- a/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
+++ b/Acompanhamento/Risk_list_Sistema de Rastreamentol.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Magnitude</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>Organizar os treinamentos aos Sábados para não gerar aumento de custo significativo ao projeto</t>
+  </si>
+  <si>
+    <t>Risco de não terminar as atividades em tempo hábil para a entrega final do projeto</t>
+  </si>
+  <si>
+    <t>sempre realizar atualizações dos documentos de forma rotineira e não deixar muitas atualizações pra um tempo curto.</t>
+  </si>
+  <si>
+    <t>atualizações realizadas ao longo de toda a semana, preferencialmente todos os dias úteis.</t>
+  </si>
+  <si>
+    <t>Desenvolvedores</t>
   </si>
 </sst>
 </file>
@@ -310,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -356,6 +368,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,7 +700,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -718,7 +742,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -741,10 +765,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="94" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -855,7 +879,7 @@
         <v>0.05</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="H4:H11" si="0">+F4*G4</f>
+        <f t="shared" ref="H4:H12" si="0">+F4*G4</f>
         <v>0.25</v>
       </c>
       <c r="I4" s="7" t="s">
@@ -1091,6 +1115,34 @@
       </c>
       <c r="J11" s="17" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="51">
+      <c r="B12" s="14">
+        <v>41742</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20">
+        <v>5</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="H12" s="21">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>